<commit_message>
COMIENZO DE ACTUALIZACION DE DOCUMENTACION DEL PROYECTO SGCTIAS
</commit_message>
<xml_diff>
--- a/assets/trim 1/1_Gestion_de_proyecto/1_Cronograma_de_actividades/3_cronograma_actividades_SGC.xlsx
+++ b/assets/trim 1/1_Gestion_de_proyecto/1_Cronograma_de_actividades/3_cronograma_actividades_SGC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D2A7D56-5E7C-4FC6-A51C-4DD1D7F183C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B782815-E0DC-4858-96C6-0C0343A471F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="697" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="697" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
   <si>
     <t>&lt;Nombre Proyecto&gt;</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Organismo</t>
   </si>
   <si>
-    <t>&lt;Nombre Consejería u Organismo Autónomo&gt;</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Autor</t>
   </si>
   <si>
-    <t>&lt;Nombre de la Empresa&gt;</t>
-  </si>
-  <si>
     <t>Fecha Versión</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>Versión Inicial</t>
   </si>
   <si>
-    <t>&lt;Nombre Apellido1 Apellido2&gt;</t>
-  </si>
-  <si>
     <t>CONTROL DE DISTRIBUCIÓN</t>
   </si>
   <si>
@@ -564,6 +555,24 @@
   </si>
   <si>
     <t>Costos</t>
+  </si>
+  <si>
+    <t>SENA</t>
+  </si>
+  <si>
+    <t>SGCITAS</t>
+  </si>
+  <si>
+    <t>Jose Guerra, Maryuri Leon</t>
+  </si>
+  <si>
+    <t>05/02/2023</t>
+  </si>
+  <si>
+    <t>Maryuri Leon</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2022,7 @@
     </xf>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2445,104 +2454,79 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="62" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="63" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2552,28 +2536,56 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="23" fillId="0" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="62" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="63" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2862,7 +2874,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$L$8" horiz="1" max="100" min="1" page="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$L$8" horiz="1" max="100" min="1" page="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2931,7 +2943,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2249130</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>30767</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2985,15 +2997,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>68580</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>30</xdr:col>
-          <xdr:colOff>137160</xdr:colOff>
+          <xdr:col>22</xdr:col>
+          <xdr:colOff>51392</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3299,9 +3311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3339,9 +3351,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3374,26 +3386,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3426,26 +3421,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3621,9 +3599,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
@@ -3642,77 +3622,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-    </row>
-    <row r="5" spans="2:6" ht="14.45" thickBot="1">
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-    </row>
-    <row r="6" spans="2:6" ht="14.45" thickTop="1">
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+    </row>
+    <row r="5" spans="2:6" ht="17.25" thickBot="1">
+      <c r="B5" s="149"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+    </row>
+    <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="3"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="150" t="s">
+      <c r="B8" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="150"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="150"/>
-      <c r="F8" s="150"/>
-    </row>
-    <row r="10" spans="2:6" ht="14.45" thickBot="1"/>
-    <row r="11" spans="2:6" ht="18.600000000000001" thickTop="1">
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="177"/>
+    </row>
+    <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
+    <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="159" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="161"/>
+      <c r="C11" s="158" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="160"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="148" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C12" s="161" t="s">
+        <v>160</v>
       </c>
       <c r="D12" s="162"/>
       <c r="E12" s="162"/>
       <c r="F12" s="163"/>
     </row>
-    <row r="13" spans="2:6" ht="18.600000000000001" thickBot="1">
+    <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="161" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="162"/>
@@ -3721,201 +3701,201 @@
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="161" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="176"/>
+      <c r="E14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="148" t="s">
+      <c r="F14" s="27" t="s">
         <v>8</v>
-      </c>
-      <c r="D14" s="149"/>
-      <c r="E14" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="19.899999999999999" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" s="165" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="166"/>
       <c r="E15" s="30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="167"/>
+      <c r="D16" s="168"/>
+      <c r="E16" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="186"/>
-      <c r="D16" s="187"/>
-      <c r="E16" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="16.149999999999999" thickTop="1">
+    </row>
+    <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="4"/>
-      <c r="C17" s="188"/>
-      <c r="D17" s="188"/>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1"/>
     <row r="21" spans="2:16" ht="30" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="E21" s="155"/>
+      <c r="F21" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="D21" s="157" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="157"/>
-      <c r="F21" s="17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="18" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="158" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="158"/>
+        <v>21</v>
+      </c>
+      <c r="D22" s="156" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="156"/>
       <c r="F22" s="20" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="189"/>
-      <c r="E23" s="189"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
-      <c r="D24" s="189"/>
-      <c r="E24" s="189"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="189"/>
-      <c r="E25" s="189"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="157"/>
       <c r="F25" s="23"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
-      <c r="D26" s="189"/>
-      <c r="E26" s="189"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="157"/>
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="189"/>
-      <c r="E27" s="189"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
       <c r="F27" s="23"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="189"/>
-      <c r="E28" s="189"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
       <c r="F28" s="23"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="189"/>
-      <c r="E29" s="189"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="157"/>
       <c r="F29" s="23"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="190"/>
-      <c r="E30" s="190"/>
+      <c r="D30" s="172"/>
+      <c r="E30" s="172"/>
       <c r="F30" s="26"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
     <row r="32" spans="2:16" ht="19.899999999999999" customHeight="1">
       <c r="B32" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="151" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="152"/>
-      <c r="D34" s="152"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="153"/>
+      <c r="B34" s="173" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="175"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="191"/>
-      <c r="C35" s="192"/>
-      <c r="D35" s="192"/>
-      <c r="E35" s="192"/>
-      <c r="F35" s="193"/>
+      <c r="B35" s="151"/>
+      <c r="C35" s="152"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="153"/>
     </row>
     <row r="36" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B36" s="194"/>
-      <c r="C36" s="195"/>
-      <c r="D36" s="195"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="196"/>
+      <c r="B36" s="178"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="179"/>
+      <c r="E36" s="179"/>
+      <c r="F36" s="180"/>
       <c r="J36" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B37" s="194"/>
-      <c r="C37" s="195"/>
-      <c r="D37" s="195"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="196"/>
+      <c r="B37" s="178"/>
+      <c r="C37" s="179"/>
+      <c r="D37" s="179"/>
+      <c r="E37" s="179"/>
+      <c r="F37" s="180"/>
     </row>
     <row r="38" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B38" s="194"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="195"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="196"/>
+      <c r="B38" s="178"/>
+      <c r="C38" s="179"/>
+      <c r="D38" s="179"/>
+      <c r="E38" s="179"/>
+      <c r="F38" s="180"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="197"/>
-      <c r="C39" s="198"/>
-      <c r="D39" s="198"/>
-      <c r="E39" s="198"/>
-      <c r="F39" s="199"/>
+      <c r="B39" s="169"/>
+      <c r="C39" s="170"/>
+      <c r="D39" s="170"/>
+      <c r="E39" s="170"/>
+      <c r="F39" s="171"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="7"/>
@@ -4056,16 +4036,16 @@
       <c r="B72" s="11"/>
     </row>
     <row r="73" spans="2:2" ht="19.899999999999999" customHeight="1"/>
-    <row r="74" spans="2:2" ht="14.45">
+    <row r="74" spans="2:2">
       <c r="B74" s="11"/>
     </row>
-    <row r="76" spans="2:2" ht="14.45">
+    <row r="76" spans="2:2">
       <c r="B76" s="11"/>
     </row>
-    <row r="78" spans="2:2" ht="14.45">
+    <row r="78" spans="2:2">
       <c r="B78" s="11"/>
     </row>
-    <row r="80" spans="2:2" ht="14.45">
+    <row r="80" spans="2:2">
       <c r="B80" s="11"/>
     </row>
     <row r="81" spans="2:3">
@@ -4076,6 +4056,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
@@ -4092,18 +4084,6 @@
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -4114,16 +4094,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:BQ78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="13" ySplit="11" topLeftCell="N41" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="K45" sqref="K45"/>
+    <sheetView showGridLines="0" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane xSplit="13" ySplit="11" topLeftCell="BE13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="48" customWidth="1"/>
     <col min="2" max="2" width="68.28515625" style="32" customWidth="1"/>
@@ -4131,302 +4112,302 @@
     <col min="6" max="6" width="37.28515625" style="57" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="42" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" style="32" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="42" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="32" customWidth="1"/>
-    <col min="13" max="13" width="1.85546875" style="32" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="42" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="42" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="42" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="32" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" style="32" customWidth="1"/>
     <col min="14" max="69" width="2.42578125" style="32" customWidth="1"/>
     <col min="70" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:69" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="175"/>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
-      <c r="Q1" s="175"/>
-      <c r="R1" s="175"/>
-      <c r="S1" s="175"/>
-      <c r="T1" s="175"/>
-      <c r="U1" s="175"/>
-      <c r="V1" s="175"/>
-      <c r="W1" s="175"/>
-      <c r="X1" s="175"/>
-      <c r="Y1" s="175"/>
-      <c r="Z1" s="175"/>
-      <c r="AA1" s="175"/>
-      <c r="AB1" s="175"/>
-      <c r="AC1" s="175"/>
-      <c r="AD1" s="175"/>
-      <c r="AE1" s="175"/>
-      <c r="AF1" s="175"/>
-      <c r="AG1" s="175"/>
-      <c r="AH1" s="175"/>
-      <c r="AI1" s="175"/>
-      <c r="AJ1" s="175"/>
-      <c r="AK1" s="175"/>
-      <c r="AL1" s="175"/>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="175"/>
-      <c r="AO1" s="175"/>
-      <c r="AP1" s="175"/>
-      <c r="AQ1" s="175"/>
-      <c r="AR1" s="175"/>
-      <c r="AS1" s="175"/>
-      <c r="AT1" s="175"/>
-      <c r="AU1" s="175"/>
-      <c r="AV1" s="175"/>
-      <c r="AW1" s="175"/>
-      <c r="AX1" s="175"/>
-      <c r="AY1" s="175"/>
-      <c r="AZ1" s="175"/>
-      <c r="BA1" s="175"/>
-      <c r="BB1" s="175"/>
-      <c r="BC1" s="175"/>
-      <c r="BD1" s="175"/>
-      <c r="BE1" s="175"/>
-      <c r="BF1" s="175"/>
-      <c r="BG1" s="175"/>
-      <c r="BH1" s="175"/>
-      <c r="BI1" s="175"/>
-      <c r="BJ1" s="175"/>
-      <c r="BK1" s="175"/>
-      <c r="BL1" s="175"/>
-      <c r="BM1" s="175"/>
-      <c r="BN1" s="175"/>
-      <c r="BO1" s="175"/>
-      <c r="BP1" s="175"/>
-      <c r="BQ1" s="175"/>
+      <c r="A1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+      <c r="N1" s="186"/>
+      <c r="O1" s="186"/>
+      <c r="P1" s="186"/>
+      <c r="Q1" s="186"/>
+      <c r="R1" s="186"/>
+      <c r="S1" s="186"/>
+      <c r="T1" s="186"/>
+      <c r="U1" s="186"/>
+      <c r="V1" s="186"/>
+      <c r="W1" s="186"/>
+      <c r="X1" s="186"/>
+      <c r="Y1" s="186"/>
+      <c r="Z1" s="186"/>
+      <c r="AA1" s="186"/>
+      <c r="AB1" s="186"/>
+      <c r="AC1" s="186"/>
+      <c r="AD1" s="186"/>
+      <c r="AE1" s="186"/>
+      <c r="AF1" s="186"/>
+      <c r="AG1" s="186"/>
+      <c r="AH1" s="186"/>
+      <c r="AI1" s="186"/>
+      <c r="AJ1" s="186"/>
+      <c r="AK1" s="186"/>
+      <c r="AL1" s="186"/>
+      <c r="AM1" s="186"/>
+      <c r="AN1" s="186"/>
+      <c r="AO1" s="186"/>
+      <c r="AP1" s="186"/>
+      <c r="AQ1" s="186"/>
+      <c r="AR1" s="186"/>
+      <c r="AS1" s="186"/>
+      <c r="AT1" s="186"/>
+      <c r="AU1" s="186"/>
+      <c r="AV1" s="186"/>
+      <c r="AW1" s="186"/>
+      <c r="AX1" s="186"/>
+      <c r="AY1" s="186"/>
+      <c r="AZ1" s="186"/>
+      <c r="BA1" s="186"/>
+      <c r="BB1" s="186"/>
+      <c r="BC1" s="186"/>
+      <c r="BD1" s="186"/>
+      <c r="BE1" s="186"/>
+      <c r="BF1" s="186"/>
+      <c r="BG1" s="186"/>
+      <c r="BH1" s="186"/>
+      <c r="BI1" s="186"/>
+      <c r="BJ1" s="186"/>
+      <c r="BK1" s="186"/>
+      <c r="BL1" s="186"/>
+      <c r="BM1" s="186"/>
+      <c r="BN1" s="186"/>
+      <c r="BO1" s="186"/>
+      <c r="BP1" s="186"/>
+      <c r="BQ1" s="186"/>
     </row>
     <row r="2" spans="1:69" s="60" customFormat="1" ht="20.25">
-      <c r="A2" s="176" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-      <c r="Q2" s="176"/>
-      <c r="R2" s="176"/>
-      <c r="S2" s="176"/>
-      <c r="T2" s="176"/>
-      <c r="U2" s="176"/>
-      <c r="V2" s="176"/>
-      <c r="W2" s="176"/>
-      <c r="X2" s="176"/>
-      <c r="Y2" s="176"/>
-      <c r="Z2" s="176"/>
-      <c r="AA2" s="176"/>
-      <c r="AB2" s="176"/>
-      <c r="AC2" s="176"/>
-      <c r="AD2" s="176"/>
-      <c r="AE2" s="176"/>
-      <c r="AF2" s="176"/>
-      <c r="AG2" s="176"/>
-      <c r="AH2" s="176"/>
-      <c r="AI2" s="176"/>
-      <c r="AJ2" s="176"/>
-      <c r="AK2" s="176"/>
-      <c r="AL2" s="176"/>
-      <c r="AM2" s="176"/>
-      <c r="AN2" s="176"/>
-      <c r="AO2" s="176"/>
-      <c r="AP2" s="176"/>
-      <c r="AQ2" s="176"/>
-      <c r="AR2" s="176"/>
-      <c r="AS2" s="176"/>
-      <c r="AT2" s="176"/>
-      <c r="AU2" s="176"/>
-      <c r="AV2" s="176"/>
-      <c r="AW2" s="176"/>
-      <c r="AX2" s="176"/>
-      <c r="AY2" s="176"/>
-      <c r="AZ2" s="176"/>
-      <c r="BA2" s="176"/>
-      <c r="BB2" s="176"/>
-      <c r="BC2" s="176"/>
-      <c r="BD2" s="176"/>
-      <c r="BE2" s="176"/>
-      <c r="BF2" s="176"/>
-      <c r="BG2" s="176"/>
-      <c r="BH2" s="176"/>
-      <c r="BI2" s="176"/>
-      <c r="BJ2" s="176"/>
-      <c r="BK2" s="176"/>
-      <c r="BL2" s="176"/>
-      <c r="BM2" s="176"/>
-      <c r="BN2" s="176"/>
-      <c r="BO2" s="176"/>
-      <c r="BP2" s="176"/>
-      <c r="BQ2" s="176"/>
+      <c r="A2" s="187" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+      <c r="Q2" s="187"/>
+      <c r="R2" s="187"/>
+      <c r="S2" s="187"/>
+      <c r="T2" s="187"/>
+      <c r="U2" s="187"/>
+      <c r="V2" s="187"/>
+      <c r="W2" s="187"/>
+      <c r="X2" s="187"/>
+      <c r="Y2" s="187"/>
+      <c r="Z2" s="187"/>
+      <c r="AA2" s="187"/>
+      <c r="AB2" s="187"/>
+      <c r="AC2" s="187"/>
+      <c r="AD2" s="187"/>
+      <c r="AE2" s="187"/>
+      <c r="AF2" s="187"/>
+      <c r="AG2" s="187"/>
+      <c r="AH2" s="187"/>
+      <c r="AI2" s="187"/>
+      <c r="AJ2" s="187"/>
+      <c r="AK2" s="187"/>
+      <c r="AL2" s="187"/>
+      <c r="AM2" s="187"/>
+      <c r="AN2" s="187"/>
+      <c r="AO2" s="187"/>
+      <c r="AP2" s="187"/>
+      <c r="AQ2" s="187"/>
+      <c r="AR2" s="187"/>
+      <c r="AS2" s="187"/>
+      <c r="AT2" s="187"/>
+      <c r="AU2" s="187"/>
+      <c r="AV2" s="187"/>
+      <c r="AW2" s="187"/>
+      <c r="AX2" s="187"/>
+      <c r="AY2" s="187"/>
+      <c r="AZ2" s="187"/>
+      <c r="BA2" s="187"/>
+      <c r="BB2" s="187"/>
+      <c r="BC2" s="187"/>
+      <c r="BD2" s="187"/>
+      <c r="BE2" s="187"/>
+      <c r="BF2" s="187"/>
+      <c r="BG2" s="187"/>
+      <c r="BH2" s="187"/>
+      <c r="BI2" s="187"/>
+      <c r="BJ2" s="187"/>
+      <c r="BK2" s="187"/>
+      <c r="BL2" s="187"/>
+      <c r="BM2" s="187"/>
+      <c r="BN2" s="187"/>
+      <c r="BO2" s="187"/>
+      <c r="BP2" s="187"/>
+      <c r="BQ2" s="187"/>
     </row>
     <row r="3" spans="1:69" s="60" customFormat="1" ht="20.25">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
-      <c r="Q3" s="176"/>
-      <c r="R3" s="176"/>
-      <c r="S3" s="176"/>
-      <c r="T3" s="176"/>
-      <c r="U3" s="176"/>
-      <c r="V3" s="176"/>
-      <c r="W3" s="176"/>
-      <c r="X3" s="176"/>
-      <c r="Y3" s="176"/>
-      <c r="Z3" s="176"/>
-      <c r="AA3" s="176"/>
-      <c r="AB3" s="176"/>
-      <c r="AC3" s="176"/>
-      <c r="AD3" s="176"/>
-      <c r="AE3" s="176"/>
-      <c r="AF3" s="176"/>
-      <c r="AG3" s="176"/>
-      <c r="AH3" s="176"/>
-      <c r="AI3" s="176"/>
-      <c r="AJ3" s="176"/>
-      <c r="AK3" s="176"/>
-      <c r="AL3" s="176"/>
-      <c r="AM3" s="176"/>
-      <c r="AN3" s="176"/>
-      <c r="AO3" s="176"/>
-      <c r="AP3" s="176"/>
-      <c r="AQ3" s="176"/>
-      <c r="AR3" s="176"/>
-      <c r="AS3" s="176"/>
-      <c r="AT3" s="176"/>
-      <c r="AU3" s="176"/>
-      <c r="AV3" s="176"/>
-      <c r="AW3" s="176"/>
-      <c r="AX3" s="176"/>
-      <c r="AY3" s="176"/>
-      <c r="AZ3" s="176"/>
-      <c r="BA3" s="176"/>
-      <c r="BB3" s="176"/>
-      <c r="BC3" s="176"/>
-      <c r="BD3" s="176"/>
-      <c r="BE3" s="176"/>
-      <c r="BF3" s="176"/>
-      <c r="BG3" s="176"/>
-      <c r="BH3" s="176"/>
-      <c r="BI3" s="176"/>
-      <c r="BJ3" s="176"/>
-      <c r="BK3" s="176"/>
-      <c r="BL3" s="176"/>
-      <c r="BM3" s="176"/>
-      <c r="BN3" s="176"/>
-      <c r="BO3" s="176"/>
-      <c r="BP3" s="176"/>
-      <c r="BQ3" s="176"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="187"/>
+      <c r="P3" s="187"/>
+      <c r="Q3" s="187"/>
+      <c r="R3" s="187"/>
+      <c r="S3" s="187"/>
+      <c r="T3" s="187"/>
+      <c r="U3" s="187"/>
+      <c r="V3" s="187"/>
+      <c r="W3" s="187"/>
+      <c r="X3" s="187"/>
+      <c r="Y3" s="187"/>
+      <c r="Z3" s="187"/>
+      <c r="AA3" s="187"/>
+      <c r="AB3" s="187"/>
+      <c r="AC3" s="187"/>
+      <c r="AD3" s="187"/>
+      <c r="AE3" s="187"/>
+      <c r="AF3" s="187"/>
+      <c r="AG3" s="187"/>
+      <c r="AH3" s="187"/>
+      <c r="AI3" s="187"/>
+      <c r="AJ3" s="187"/>
+      <c r="AK3" s="187"/>
+      <c r="AL3" s="187"/>
+      <c r="AM3" s="187"/>
+      <c r="AN3" s="187"/>
+      <c r="AO3" s="187"/>
+      <c r="AP3" s="187"/>
+      <c r="AQ3" s="187"/>
+      <c r="AR3" s="187"/>
+      <c r="AS3" s="187"/>
+      <c r="AT3" s="187"/>
+      <c r="AU3" s="187"/>
+      <c r="AV3" s="187"/>
+      <c r="AW3" s="187"/>
+      <c r="AX3" s="187"/>
+      <c r="AY3" s="187"/>
+      <c r="AZ3" s="187"/>
+      <c r="BA3" s="187"/>
+      <c r="BB3" s="187"/>
+      <c r="BC3" s="187"/>
+      <c r="BD3" s="187"/>
+      <c r="BE3" s="187"/>
+      <c r="BF3" s="187"/>
+      <c r="BG3" s="187"/>
+      <c r="BH3" s="187"/>
+      <c r="BI3" s="187"/>
+      <c r="BJ3" s="187"/>
+      <c r="BK3" s="187"/>
+      <c r="BL3" s="187"/>
+      <c r="BM3" s="187"/>
+      <c r="BN3" s="187"/>
+      <c r="BO3" s="187"/>
+      <c r="BP3" s="187"/>
+      <c r="BQ3" s="187"/>
     </row>
     <row r="4" spans="1:69" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A4" s="177"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="177"/>
-      <c r="V4" s="177"/>
-      <c r="W4" s="177"/>
-      <c r="X4" s="177"/>
-      <c r="Y4" s="177"/>
-      <c r="Z4" s="177"/>
-      <c r="AA4" s="177"/>
-      <c r="AB4" s="177"/>
-      <c r="AC4" s="177"/>
-      <c r="AD4" s="177"/>
-      <c r="AE4" s="177"/>
-      <c r="AF4" s="177"/>
-      <c r="AG4" s="177"/>
-      <c r="AH4" s="177"/>
-      <c r="AI4" s="177"/>
-      <c r="AJ4" s="177"/>
-      <c r="AK4" s="177"/>
-      <c r="AL4" s="177"/>
-      <c r="AM4" s="177"/>
-      <c r="AN4" s="177"/>
-      <c r="AO4" s="177"/>
-      <c r="AP4" s="177"/>
-      <c r="AQ4" s="177"/>
-      <c r="AR4" s="177"/>
-      <c r="AS4" s="177"/>
-      <c r="AT4" s="177"/>
-      <c r="AU4" s="177"/>
-      <c r="AV4" s="177"/>
-      <c r="AW4" s="177"/>
-      <c r="AX4" s="177"/>
-      <c r="AY4" s="177"/>
-      <c r="AZ4" s="177"/>
-      <c r="BA4" s="177"/>
-      <c r="BB4" s="177"/>
-      <c r="BC4" s="177"/>
-      <c r="BD4" s="177"/>
-      <c r="BE4" s="177"/>
-      <c r="BF4" s="177"/>
-      <c r="BG4" s="177"/>
-      <c r="BH4" s="177"/>
-      <c r="BI4" s="177"/>
-      <c r="BJ4" s="177"/>
-      <c r="BK4" s="177"/>
-      <c r="BL4" s="177"/>
-      <c r="BM4" s="177"/>
-      <c r="BN4" s="177"/>
-      <c r="BO4" s="177"/>
-      <c r="BP4" s="177"/>
-      <c r="BQ4" s="177"/>
+      <c r="A4" s="188"/>
+      <c r="B4" s="188"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+      <c r="K4" s="188"/>
+      <c r="L4" s="188"/>
+      <c r="M4" s="188"/>
+      <c r="N4" s="188"/>
+      <c r="O4" s="188"/>
+      <c r="P4" s="188"/>
+      <c r="Q4" s="188"/>
+      <c r="R4" s="188"/>
+      <c r="S4" s="188"/>
+      <c r="T4" s="188"/>
+      <c r="U4" s="188"/>
+      <c r="V4" s="188"/>
+      <c r="W4" s="188"/>
+      <c r="X4" s="188"/>
+      <c r="Y4" s="188"/>
+      <c r="Z4" s="188"/>
+      <c r="AA4" s="188"/>
+      <c r="AB4" s="188"/>
+      <c r="AC4" s="188"/>
+      <c r="AD4" s="188"/>
+      <c r="AE4" s="188"/>
+      <c r="AF4" s="188"/>
+      <c r="AG4" s="188"/>
+      <c r="AH4" s="188"/>
+      <c r="AI4" s="188"/>
+      <c r="AJ4" s="188"/>
+      <c r="AK4" s="188"/>
+      <c r="AL4" s="188"/>
+      <c r="AM4" s="188"/>
+      <c r="AN4" s="188"/>
+      <c r="AO4" s="188"/>
+      <c r="AP4" s="188"/>
+      <c r="AQ4" s="188"/>
+      <c r="AR4" s="188"/>
+      <c r="AS4" s="188"/>
+      <c r="AT4" s="188"/>
+      <c r="AU4" s="188"/>
+      <c r="AV4" s="188"/>
+      <c r="AW4" s="188"/>
+      <c r="AX4" s="188"/>
+      <c r="AY4" s="188"/>
+      <c r="AZ4" s="188"/>
+      <c r="BA4" s="188"/>
+      <c r="BB4" s="188"/>
+      <c r="BC4" s="188"/>
+      <c r="BD4" s="188"/>
+      <c r="BE4" s="188"/>
+      <c r="BF4" s="188"/>
+      <c r="BG4" s="188"/>
+      <c r="BH4" s="188"/>
+      <c r="BI4" s="188"/>
+      <c r="BJ4" s="188"/>
+      <c r="BK4" s="188"/>
+      <c r="BL4" s="188"/>
+      <c r="BM4" s="188"/>
+      <c r="BN4" s="188"/>
+      <c r="BO4" s="188"/>
+      <c r="BP4" s="188"/>
+      <c r="BQ4" s="188"/>
     </row>
     <row r="5" spans="1:69" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
       <c r="A5" s="59"/>
@@ -4536,7 +4517,7 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="B8" s="55" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" s="58"/>
       <c r="D8" s="185">
@@ -4547,184 +4528,184 @@
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
       <c r="K8" s="44" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L8" s="37">
         <v>1</v>
       </c>
-      <c r="N8" s="181" t="str">
+      <c r="N8" s="182" t="str">
         <f>"Semana "&amp;(N10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 1</v>
       </c>
-      <c r="O8" s="182"/>
-      <c r="P8" s="182"/>
-      <c r="Q8" s="182"/>
-      <c r="R8" s="182"/>
-      <c r="S8" s="182"/>
-      <c r="T8" s="183"/>
-      <c r="U8" s="181" t="str">
+      <c r="O8" s="183"/>
+      <c r="P8" s="183"/>
+      <c r="Q8" s="183"/>
+      <c r="R8" s="183"/>
+      <c r="S8" s="183"/>
+      <c r="T8" s="184"/>
+      <c r="U8" s="182" t="str">
         <f>"Semana "&amp;(U10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 2</v>
       </c>
-      <c r="V8" s="182"/>
-      <c r="W8" s="182"/>
-      <c r="X8" s="182"/>
-      <c r="Y8" s="182"/>
-      <c r="Z8" s="182"/>
-      <c r="AA8" s="183"/>
-      <c r="AB8" s="181" t="str">
+      <c r="V8" s="183"/>
+      <c r="W8" s="183"/>
+      <c r="X8" s="183"/>
+      <c r="Y8" s="183"/>
+      <c r="Z8" s="183"/>
+      <c r="AA8" s="184"/>
+      <c r="AB8" s="182" t="str">
         <f>"Semana "&amp;(AB10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 3</v>
       </c>
-      <c r="AC8" s="182"/>
-      <c r="AD8" s="182"/>
-      <c r="AE8" s="182"/>
-      <c r="AF8" s="182"/>
-      <c r="AG8" s="182"/>
-      <c r="AH8" s="183"/>
-      <c r="AI8" s="181" t="str">
+      <c r="AC8" s="183"/>
+      <c r="AD8" s="183"/>
+      <c r="AE8" s="183"/>
+      <c r="AF8" s="183"/>
+      <c r="AG8" s="183"/>
+      <c r="AH8" s="184"/>
+      <c r="AI8" s="182" t="str">
         <f>"Semana "&amp;(AI10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 4</v>
       </c>
-      <c r="AJ8" s="182"/>
-      <c r="AK8" s="182"/>
-      <c r="AL8" s="182"/>
-      <c r="AM8" s="182"/>
-      <c r="AN8" s="182"/>
-      <c r="AO8" s="183"/>
-      <c r="AP8" s="181" t="str">
+      <c r="AJ8" s="183"/>
+      <c r="AK8" s="183"/>
+      <c r="AL8" s="183"/>
+      <c r="AM8" s="183"/>
+      <c r="AN8" s="183"/>
+      <c r="AO8" s="184"/>
+      <c r="AP8" s="182" t="str">
         <f>"Semana "&amp;(AP10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 5</v>
       </c>
-      <c r="AQ8" s="182"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
-      <c r="AU8" s="182"/>
-      <c r="AV8" s="183"/>
-      <c r="AW8" s="181" t="str">
+      <c r="AQ8" s="183"/>
+      <c r="AR8" s="183"/>
+      <c r="AS8" s="183"/>
+      <c r="AT8" s="183"/>
+      <c r="AU8" s="183"/>
+      <c r="AV8" s="184"/>
+      <c r="AW8" s="182" t="str">
         <f>"Semana "&amp;(AW10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 6</v>
       </c>
-      <c r="AX8" s="182"/>
-      <c r="AY8" s="182"/>
-      <c r="AZ8" s="182"/>
-      <c r="BA8" s="182"/>
-      <c r="BB8" s="182"/>
-      <c r="BC8" s="183"/>
-      <c r="BD8" s="181" t="str">
+      <c r="AX8" s="183"/>
+      <c r="AY8" s="183"/>
+      <c r="AZ8" s="183"/>
+      <c r="BA8" s="183"/>
+      <c r="BB8" s="183"/>
+      <c r="BC8" s="184"/>
+      <c r="BD8" s="182" t="str">
         <f>"Semana "&amp;(BD10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 7</v>
       </c>
-      <c r="BE8" s="182"/>
-      <c r="BF8" s="182"/>
-      <c r="BG8" s="182"/>
-      <c r="BH8" s="182"/>
-      <c r="BI8" s="182"/>
-      <c r="BJ8" s="183"/>
-      <c r="BK8" s="181" t="str">
+      <c r="BE8" s="183"/>
+      <c r="BF8" s="183"/>
+      <c r="BG8" s="183"/>
+      <c r="BH8" s="183"/>
+      <c r="BI8" s="183"/>
+      <c r="BJ8" s="184"/>
+      <c r="BK8" s="182" t="str">
         <f>"Semana "&amp;(BK10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 8</v>
       </c>
-      <c r="BL8" s="182"/>
-      <c r="BM8" s="182"/>
-      <c r="BN8" s="182"/>
-      <c r="BO8" s="182"/>
-      <c r="BP8" s="182"/>
-      <c r="BQ8" s="183"/>
+      <c r="BL8" s="183"/>
+      <c r="BM8" s="183"/>
+      <c r="BN8" s="183"/>
+      <c r="BO8" s="183"/>
+      <c r="BP8" s="183"/>
+      <c r="BQ8" s="184"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="B9" s="55" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="58"/>
-      <c r="D9" s="184" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
+      <c r="D9" s="181" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
       <c r="G9" s="46"/>
       <c r="H9" s="46"/>
-      <c r="N9" s="178">
+      <c r="N9" s="189">
         <f>N10</f>
         <v>44963</v>
       </c>
-      <c r="O9" s="179"/>
-      <c r="P9" s="179"/>
-      <c r="Q9" s="179"/>
-      <c r="R9" s="179"/>
-      <c r="S9" s="179"/>
-      <c r="T9" s="180"/>
-      <c r="U9" s="178">
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="191"/>
+      <c r="U9" s="189">
         <f>U10</f>
         <v>44970</v>
       </c>
-      <c r="V9" s="179"/>
-      <c r="W9" s="179"/>
-      <c r="X9" s="179"/>
-      <c r="Y9" s="179"/>
-      <c r="Z9" s="179"/>
-      <c r="AA9" s="180"/>
-      <c r="AB9" s="178">
+      <c r="V9" s="190"/>
+      <c r="W9" s="190"/>
+      <c r="X9" s="190"/>
+      <c r="Y9" s="190"/>
+      <c r="Z9" s="190"/>
+      <c r="AA9" s="191"/>
+      <c r="AB9" s="189">
         <f>AB10</f>
         <v>44977</v>
       </c>
-      <c r="AC9" s="179"/>
-      <c r="AD9" s="179"/>
-      <c r="AE9" s="179"/>
-      <c r="AF9" s="179"/>
-      <c r="AG9" s="179"/>
-      <c r="AH9" s="180"/>
-      <c r="AI9" s="178">
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="191"/>
+      <c r="AI9" s="189">
         <f>AI10</f>
         <v>44984</v>
       </c>
-      <c r="AJ9" s="179"/>
-      <c r="AK9" s="179"/>
-      <c r="AL9" s="179"/>
-      <c r="AM9" s="179"/>
-      <c r="AN9" s="179"/>
-      <c r="AO9" s="180"/>
-      <c r="AP9" s="178">
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="191"/>
+      <c r="AP9" s="189">
         <f>AP10</f>
         <v>44991</v>
       </c>
-      <c r="AQ9" s="179"/>
-      <c r="AR9" s="179"/>
-      <c r="AS9" s="179"/>
-      <c r="AT9" s="179"/>
-      <c r="AU9" s="179"/>
-      <c r="AV9" s="180"/>
-      <c r="AW9" s="178">
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="190"/>
+      <c r="AS9" s="190"/>
+      <c r="AT9" s="190"/>
+      <c r="AU9" s="190"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="189">
         <f>AW10</f>
         <v>44998</v>
       </c>
-      <c r="AX9" s="179"/>
-      <c r="AY9" s="179"/>
-      <c r="AZ9" s="179"/>
-      <c r="BA9" s="179"/>
-      <c r="BB9" s="179"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="178">
+      <c r="AX9" s="190"/>
+      <c r="AY9" s="190"/>
+      <c r="AZ9" s="190"/>
+      <c r="BA9" s="190"/>
+      <c r="BB9" s="190"/>
+      <c r="BC9" s="191"/>
+      <c r="BD9" s="189">
         <f>BD10</f>
         <v>45005</v>
       </c>
-      <c r="BE9" s="179"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BH9" s="179"/>
-      <c r="BI9" s="179"/>
-      <c r="BJ9" s="180"/>
-      <c r="BK9" s="178">
+      <c r="BE9" s="190"/>
+      <c r="BF9" s="190"/>
+      <c r="BG9" s="190"/>
+      <c r="BH9" s="190"/>
+      <c r="BI9" s="190"/>
+      <c r="BJ9" s="191"/>
+      <c r="BK9" s="189">
         <f>BK10</f>
         <v>45012</v>
       </c>
-      <c r="BL9" s="179"/>
-      <c r="BM9" s="179"/>
-      <c r="BN9" s="179"/>
-      <c r="BO9" s="179"/>
-      <c r="BP9" s="179"/>
-      <c r="BQ9" s="180"/>
+      <c r="BL9" s="190"/>
+      <c r="BM9" s="190"/>
+      <c r="BN9" s="190"/>
+      <c r="BO9" s="190"/>
+      <c r="BP9" s="190"/>
+      <c r="BQ9" s="191"/>
     </row>
     <row r="10" spans="1:69">
       <c r="N10" s="38">
@@ -4954,40 +4935,40 @@
     </row>
     <row r="11" spans="1:69" s="147" customFormat="1" ht="27.75" customHeight="1">
       <c r="A11" s="142" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="142" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="142" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="142" t="s">
+      <c r="E11" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="142" t="s">
+      <c r="F11" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="142" t="s">
+      <c r="G11" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="142" t="s">
+      <c r="H11" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="143" t="s">
+      <c r="I11" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="143" t="s">
+      <c r="J11" s="142" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="143" t="s">
+      <c r="K11" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="142" t="s">
+      <c r="L11" s="143" t="s">
         <v>41</v>
-      </c>
-      <c r="J11" s="142" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="143" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="143" t="s">
-        <v>44</v>
       </c>
       <c r="M11" s="143"/>
       <c r="N11" s="144" t="str">
@@ -5215,22 +5196,22 @@
         <v>D</v>
       </c>
     </row>
-    <row r="12" spans="1:69" s="71" customFormat="1" ht="27" customHeight="1">
+    <row r="12" spans="1:69" s="71" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A12" s="97" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="62" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F12" s="62"/>
       <c r="G12" s="62"/>
@@ -5302,26 +5283,26 @@
     </row>
     <row r="13" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="134" t="str">
-        <f t="shared" ref="A13:A28" ca="1" si="44">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A13:A28" si="44">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B13" s="89" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="90" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="90">
         <v>2</v>
       </c>
       <c r="E13" s="90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" s="90" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H13" s="92"/>
       <c r="I13" s="93">
@@ -5396,25 +5377,25 @@
     </row>
     <row r="14" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A14" s="133" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="103" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="90">
         <v>2</v>
       </c>
       <c r="E14" s="90" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F14" s="105" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G14" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H14" s="106"/>
       <c r="I14" s="137">
@@ -5489,25 +5470,25 @@
     </row>
     <row r="15" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A15" s="133" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" s="103" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="90">
         <v>2</v>
       </c>
       <c r="E15" s="90" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F15" s="105" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G15" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H15" s="106"/>
       <c r="I15" s="137">
@@ -5582,25 +5563,25 @@
     </row>
     <row r="16" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="133" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B16" s="103" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="90">
         <v>2</v>
       </c>
       <c r="E16" s="90" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="105" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G16" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" s="106"/>
       <c r="I16" s="137">
@@ -5675,25 +5656,25 @@
     </row>
     <row r="17" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A17" s="133" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" s="103" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17" s="136" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" s="90">
         <v>2</v>
       </c>
       <c r="E17" s="90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F17" s="105" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G17" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17" s="106"/>
       <c r="I17" s="137">
@@ -5768,23 +5749,23 @@
     </row>
     <row r="18" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A18" s="133" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="103" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C18" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D18" s="104">
         <v>3</v>
       </c>
       <c r="E18" s="112"/>
       <c r="F18" s="105" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G18" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H18" s="106"/>
       <c r="I18" s="140">
@@ -5805,7 +5786,7 @@
       <c r="P18" s="76"/>
       <c r="Q18" s="76"/>
       <c r="R18" s="76"/>
-      <c r="S18" s="76"/>
+      <c r="S18" s="200"/>
       <c r="T18" s="76"/>
       <c r="U18" s="76"/>
       <c r="V18" s="76"/>
@@ -5857,27 +5838,27 @@
       <c r="BP18" s="76"/>
       <c r="BQ18" s="78"/>
     </row>
-    <row r="19" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="19" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A19" s="133" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" s="105" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C19" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D19" s="104">
         <v>1</v>
       </c>
       <c r="E19" s="104" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F19" s="105" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G19" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H19" s="106"/>
       <c r="I19" s="107">
@@ -5950,15 +5931,15 @@
       <c r="BP19" s="76"/>
       <c r="BQ19" s="78"/>
     </row>
-    <row r="20" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="20" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A20" s="133" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B20" s="105" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D20" s="104">
         <v>1</v>
@@ -5967,10 +5948,10 @@
         <v>1.2</v>
       </c>
       <c r="F20" s="105" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G20" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H20" s="106"/>
       <c r="I20" s="107">
@@ -6043,29 +6024,29 @@
       <c r="BP20" s="76"/>
       <c r="BQ20" s="78"/>
     </row>
-    <row r="21" spans="1:69" s="71" customFormat="1" ht="27" customHeight="1">
+    <row r="21" spans="1:69" s="71" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A21" s="97" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
       <c r="B21" s="123" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F21" s="69"/>
       <c r="G21" s="63"/>
       <c r="H21" s="63"/>
       <c r="I21" s="64"/>
       <c r="J21" s="64" t="str">
-        <f t="shared" ref="J21:J46" si="45">IF(ISBLANK(I21)," - ",IF(K21=0,I21,I21+K21-1))</f>
+        <f t="shared" ref="J21" si="45">IF(ISBLANK(I21)," - ",IF(K21=0,I21,I21+K21-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K21" s="65"/>
@@ -6130,14 +6111,14 @@
     </row>
     <row r="22" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A22" s="88" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B22" s="89" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" s="90" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" s="90">
         <v>3</v>
@@ -6146,10 +6127,10 @@
         <v>3.1</v>
       </c>
       <c r="F22" s="91" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G22" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H22" s="92"/>
       <c r="I22" s="93">
@@ -6224,26 +6205,26 @@
     </row>
     <row r="23" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A23" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.2</v>
       </c>
       <c r="B23" s="103" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" s="135" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="104">
         <v>1</v>
       </c>
       <c r="E23" s="104" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F23" s="105" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G23" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H23" s="106"/>
       <c r="I23" s="137">
@@ -6318,26 +6299,26 @@
     </row>
     <row r="24" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A24" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.3</v>
       </c>
       <c r="B24" s="103" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C24" s="135" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" s="104">
         <v>1</v>
       </c>
       <c r="E24" s="104" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" s="105" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G24" s="136" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H24" s="106"/>
       <c r="I24" s="137">
@@ -6410,16 +6391,16 @@
       <c r="BP24" s="76"/>
       <c r="BQ24" s="78"/>
     </row>
-    <row r="25" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="25" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A25" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.4</v>
       </c>
       <c r="B25" s="103" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D25" s="104">
         <v>2</v>
@@ -6428,10 +6409,10 @@
         <v>2.4</v>
       </c>
       <c r="F25" s="105" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G25" s="136" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H25" s="106"/>
       <c r="I25" s="107">
@@ -6506,14 +6487,14 @@
     </row>
     <row r="26" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A26" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.5</v>
       </c>
       <c r="B26" s="105" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C26" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" s="104">
         <v>2</v>
@@ -6525,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="135" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H26" s="106"/>
       <c r="I26" s="137">
@@ -6600,26 +6581,26 @@
     </row>
     <row r="27" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A27" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.6</v>
       </c>
       <c r="B27" s="103" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C27" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D27" s="104">
         <v>1</v>
       </c>
       <c r="E27" s="104" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F27" s="105" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G27" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H27" s="106"/>
       <c r="I27" s="107">
@@ -6694,26 +6675,26 @@
     </row>
     <row r="28" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A28" s="102" t="str">
-        <f t="shared" ca="1" si="44"/>
+        <f t="shared" si="44"/>
         <v>2.7</v>
       </c>
       <c r="B28" s="103" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D28" s="104">
         <v>1</v>
       </c>
       <c r="E28" s="104" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F28" s="105" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G28" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H28" s="106"/>
       <c r="I28" s="141">
@@ -6786,15 +6767,15 @@
       <c r="BP28" s="76"/>
       <c r="BQ28" s="78"/>
     </row>
-    <row r="29" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="29" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A29" s="102" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B29" s="103" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C29" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D29" s="104">
         <v>3</v>
@@ -6803,10 +6784,10 @@
         <v>3.6</v>
       </c>
       <c r="F29" s="105" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G29" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H29" s="106"/>
       <c r="I29" s="107">
@@ -6879,27 +6860,27 @@
       <c r="BP29" s="84"/>
       <c r="BQ29" s="85"/>
     </row>
-    <row r="30" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="30" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A30" s="102" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B30" s="103" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C30" s="104" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D30" s="104">
         <v>3</v>
       </c>
       <c r="E30" s="104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F30" s="105" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G30" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H30" s="106"/>
       <c r="I30" s="107">
@@ -6972,27 +6953,27 @@
       <c r="BP30" s="76"/>
       <c r="BQ30" s="78"/>
     </row>
-    <row r="31" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="31" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A31" s="102" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B31" s="114" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C31" s="115" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D31" s="115">
         <v>3</v>
       </c>
       <c r="E31" s="115" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F31" s="116" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H31" s="117"/>
       <c r="I31" s="118">
@@ -7065,22 +7046,22 @@
       <c r="BP31" s="76"/>
       <c r="BQ31" s="78"/>
     </row>
-    <row r="32" spans="1:69" s="71" customFormat="1" ht="27" customHeight="1">
+    <row r="32" spans="1:69" s="71" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A32" s="97" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
       <c r="B32" s="123" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C32" s="62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D32" s="62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E32" s="62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F32" s="69"/>
       <c r="G32" s="63"/>
@@ -7147,28 +7128,28 @@
       <c r="BP32" s="86"/>
       <c r="BQ32" s="87"/>
     </row>
-    <row r="33" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="33" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A33" s="88" t="str">
-        <f t="shared" ref="A33:A38" ca="1" si="46">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A33:A38" si="46">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B33" s="89" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C33" s="90" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D33" s="90">
         <v>1</v>
       </c>
       <c r="E33" s="90" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F33" s="91" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G33" s="90" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H33" s="92"/>
       <c r="I33" s="107">
@@ -7241,28 +7222,28 @@
       <c r="BP33" s="76"/>
       <c r="BQ33" s="78"/>
     </row>
-    <row r="34" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="34" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A34" s="102" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" si="46"/>
         <v>3.2</v>
       </c>
       <c r="B34" s="103" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C34" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D34" s="104">
         <v>1</v>
       </c>
       <c r="E34" s="104" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F34" s="105" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G34" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H34" s="106"/>
       <c r="I34" s="107">
@@ -7335,28 +7316,28 @@
       <c r="BP34" s="76"/>
       <c r="BQ34" s="78"/>
     </row>
-    <row r="35" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="35" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A35" s="102" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" si="46"/>
         <v>3.3</v>
       </c>
       <c r="B35" s="103" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C35" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D35" s="104">
         <v>1</v>
       </c>
       <c r="E35" s="104" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F35" s="105" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G35" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H35" s="106"/>
       <c r="I35" s="107">
@@ -7431,26 +7412,26 @@
     </row>
     <row r="36" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
       <c r="A36" s="102" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" si="46"/>
         <v>3.4</v>
       </c>
       <c r="B36" s="103" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C36" s="104" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D36" s="104">
         <v>1</v>
       </c>
       <c r="E36" s="104" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F36" s="105" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G36" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H36" s="106"/>
       <c r="I36" s="107">
@@ -7523,28 +7504,28 @@
       <c r="BP36" s="76"/>
       <c r="BQ36" s="78"/>
     </row>
-    <row r="37" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="37" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A37" s="102" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" si="46"/>
         <v>3.5</v>
       </c>
       <c r="B37" s="103" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C37" s="104" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D37" s="104">
         <v>1</v>
       </c>
       <c r="E37" s="104" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F37" s="105" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G37" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H37" s="106"/>
       <c r="I37" s="107">
@@ -7617,28 +7598,28 @@
       <c r="BP37" s="76"/>
       <c r="BQ37" s="78"/>
     </row>
-    <row r="38" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="38" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A38" s="102" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" si="46"/>
         <v>3.6</v>
       </c>
       <c r="B38" s="103" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C38" s="104" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38" s="104">
         <v>3</v>
       </c>
       <c r="E38" s="104" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F38" s="105" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G38" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H38" s="106"/>
       <c r="I38" s="107">
@@ -7711,28 +7692,28 @@
       <c r="BP38" s="76"/>
       <c r="BQ38" s="78"/>
     </row>
-    <row r="39" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="39" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A39" s="113" t="str">
-        <f t="shared" ref="A39" ca="1" si="47">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A39" si="47">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.7</v>
       </c>
       <c r="B39" s="114" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D39" s="115">
         <v>3</v>
       </c>
       <c r="E39" s="115" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F39" s="116" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G39" s="115" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H39" s="117"/>
       <c r="I39" s="118">
@@ -7805,22 +7786,22 @@
       <c r="BP39" s="84"/>
       <c r="BQ39" s="85"/>
     </row>
-    <row r="40" spans="1:69" s="71" customFormat="1" ht="27" customHeight="1">
+    <row r="40" spans="1:69" s="71" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A40" s="97" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
       <c r="B40" s="123" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C40" s="62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D40" s="62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E40" s="62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F40" s="69"/>
       <c r="G40" s="63"/>
@@ -7887,27 +7868,27 @@
       <c r="BP40" s="86"/>
       <c r="BQ40" s="87"/>
     </row>
-    <row r="41" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="41" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A41" s="88" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B41" s="89" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C41" s="90" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D41" s="90">
         <v>3</v>
       </c>
       <c r="E41" s="90" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F41" s="91" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G41" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H41" s="92"/>
       <c r="I41" s="93">
@@ -7980,27 +7961,27 @@
       <c r="BP41" s="76"/>
       <c r="BQ41" s="78"/>
     </row>
-    <row r="42" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="42" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A42" s="88" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B42" s="103" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C42" s="104" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D42" s="104">
         <v>3</v>
       </c>
       <c r="E42" s="104" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F42" s="105" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G42" s="115" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H42" s="106"/>
       <c r="I42" s="107">
@@ -8073,27 +8054,27 @@
       <c r="BP42" s="76"/>
       <c r="BQ42" s="78"/>
     </row>
-    <row r="43" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="43" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A43" s="88" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B43" s="103" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C43" s="104" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D43" s="104">
         <v>1</v>
       </c>
       <c r="E43" s="104" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F43" s="105" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G43" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H43" s="106"/>
       <c r="I43" s="107">
@@ -8166,27 +8147,27 @@
       <c r="BP43" s="76"/>
       <c r="BQ43" s="78"/>
     </row>
-    <row r="44" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="44" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A44" s="88" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B44" s="103" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C44" s="104" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D44" s="104">
         <v>3</v>
       </c>
       <c r="E44" s="104" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F44" s="105" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G44" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H44" s="106"/>
       <c r="I44" s="107">
@@ -8259,27 +8240,27 @@
       <c r="BP44" s="76"/>
       <c r="BQ44" s="78"/>
     </row>
-    <row r="45" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="45" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A45" s="88" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B45" s="103" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C45" s="104" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D45" s="104">
         <v>3</v>
       </c>
       <c r="E45" s="104" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F45" s="105" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G45" s="104" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H45" s="106"/>
       <c r="I45" s="107">
@@ -8352,27 +8333,27 @@
       <c r="BP45" s="76"/>
       <c r="BQ45" s="78"/>
     </row>
-    <row r="46" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="46" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A46" s="88" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B46" s="103" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C46" s="104" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D46" s="104">
         <v>3</v>
       </c>
       <c r="E46" s="104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F46" s="105" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G46" s="104" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H46" s="106"/>
       <c r="I46" s="107">
@@ -8445,27 +8426,27 @@
       <c r="BP46" s="76"/>
       <c r="BQ46" s="78"/>
     </row>
-    <row r="47" spans="1:69" s="75" customFormat="1" ht="27" customHeight="1">
+    <row r="47" spans="1:69" s="75" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A47" s="88" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B47" s="114" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C47" s="115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D47" s="115">
         <v>3</v>
       </c>
       <c r="E47" s="115" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F47" s="116" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G47" s="115" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H47" s="117"/>
       <c r="I47" s="118">
@@ -8538,471 +8519,471 @@
       <c r="BP47" s="76"/>
       <c r="BQ47" s="78"/>
     </row>
-    <row r="48" spans="1:69" ht="60" customHeight="1"/>
+    <row r="48" spans="1:69" ht="60" hidden="1" customHeight="1"/>
     <row r="49" spans="1:69" ht="60" customHeight="1"/>
     <row r="50" spans="1:69">
       <c r="A50" s="51" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
-      <c r="B50" s="167" t="s">
-        <v>142</v>
-      </c>
-      <c r="C50" s="167"/>
-      <c r="D50" s="167"/>
-      <c r="E50" s="167"/>
-      <c r="F50" s="167"/>
-      <c r="G50" s="167"/>
-      <c r="H50" s="167"/>
-      <c r="I50" s="167"/>
-      <c r="J50" s="167"/>
-      <c r="K50" s="167"/>
-      <c r="L50" s="167"/>
-      <c r="M50" s="167"/>
-      <c r="N50" s="167"/>
-      <c r="O50" s="167"/>
-      <c r="P50" s="167"/>
-      <c r="Q50" s="167"/>
-      <c r="R50" s="167"/>
-      <c r="S50" s="167"/>
-      <c r="T50" s="167"/>
-      <c r="U50" s="167"/>
-      <c r="V50" s="167"/>
-      <c r="W50" s="167"/>
-      <c r="X50" s="167"/>
-      <c r="Y50" s="167"/>
-      <c r="Z50" s="167"/>
-      <c r="AA50" s="167"/>
-      <c r="AB50" s="167"/>
-      <c r="AC50" s="167"/>
-      <c r="AD50" s="167"/>
-      <c r="AE50" s="167"/>
-      <c r="AF50" s="167"/>
-      <c r="AG50" s="167"/>
-      <c r="AH50" s="167"/>
-      <c r="AI50" s="167"/>
-      <c r="AJ50" s="167"/>
-      <c r="AK50" s="167"/>
-      <c r="AL50" s="167"/>
-      <c r="AM50" s="167"/>
-      <c r="AN50" s="167"/>
-      <c r="AO50" s="167"/>
-      <c r="AP50" s="167"/>
-      <c r="AQ50" s="167"/>
-      <c r="AR50" s="167"/>
-      <c r="AS50" s="167"/>
-      <c r="AT50" s="167"/>
-      <c r="AU50" s="167"/>
-      <c r="AV50" s="167"/>
-      <c r="AW50" s="167"/>
-      <c r="AX50" s="167"/>
-      <c r="AY50" s="167"/>
-      <c r="AZ50" s="167"/>
-      <c r="BA50" s="167"/>
-      <c r="BB50" s="167"/>
-      <c r="BC50" s="167"/>
-      <c r="BD50" s="167"/>
-      <c r="BE50" s="167"/>
-      <c r="BF50" s="167"/>
-      <c r="BG50" s="167"/>
-      <c r="BH50" s="167"/>
-      <c r="BI50" s="167"/>
-      <c r="BJ50" s="167"/>
-      <c r="BK50" s="167"/>
-      <c r="BL50" s="167"/>
-      <c r="BM50" s="167"/>
-      <c r="BN50" s="167"/>
-      <c r="BO50" s="167"/>
-      <c r="BP50" s="167"/>
-      <c r="BQ50" s="168"/>
+      <c r="B50" s="192" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="192"/>
+      <c r="D50" s="192"/>
+      <c r="E50" s="192"/>
+      <c r="F50" s="192"/>
+      <c r="G50" s="192"/>
+      <c r="H50" s="192"/>
+      <c r="I50" s="192"/>
+      <c r="J50" s="192"/>
+      <c r="K50" s="192"/>
+      <c r="L50" s="192"/>
+      <c r="M50" s="192"/>
+      <c r="N50" s="192"/>
+      <c r="O50" s="192"/>
+      <c r="P50" s="192"/>
+      <c r="Q50" s="192"/>
+      <c r="R50" s="192"/>
+      <c r="S50" s="192"/>
+      <c r="T50" s="192"/>
+      <c r="U50" s="192"/>
+      <c r="V50" s="192"/>
+      <c r="W50" s="192"/>
+      <c r="X50" s="192"/>
+      <c r="Y50" s="192"/>
+      <c r="Z50" s="192"/>
+      <c r="AA50" s="192"/>
+      <c r="AB50" s="192"/>
+      <c r="AC50" s="192"/>
+      <c r="AD50" s="192"/>
+      <c r="AE50" s="192"/>
+      <c r="AF50" s="192"/>
+      <c r="AG50" s="192"/>
+      <c r="AH50" s="192"/>
+      <c r="AI50" s="192"/>
+      <c r="AJ50" s="192"/>
+      <c r="AK50" s="192"/>
+      <c r="AL50" s="192"/>
+      <c r="AM50" s="192"/>
+      <c r="AN50" s="192"/>
+      <c r="AO50" s="192"/>
+      <c r="AP50" s="192"/>
+      <c r="AQ50" s="192"/>
+      <c r="AR50" s="192"/>
+      <c r="AS50" s="192"/>
+      <c r="AT50" s="192"/>
+      <c r="AU50" s="192"/>
+      <c r="AV50" s="192"/>
+      <c r="AW50" s="192"/>
+      <c r="AX50" s="192"/>
+      <c r="AY50" s="192"/>
+      <c r="AZ50" s="192"/>
+      <c r="BA50" s="192"/>
+      <c r="BB50" s="192"/>
+      <c r="BC50" s="192"/>
+      <c r="BD50" s="192"/>
+      <c r="BE50" s="192"/>
+      <c r="BF50" s="192"/>
+      <c r="BG50" s="192"/>
+      <c r="BH50" s="192"/>
+      <c r="BI50" s="192"/>
+      <c r="BJ50" s="192"/>
+      <c r="BK50" s="192"/>
+      <c r="BL50" s="192"/>
+      <c r="BM50" s="192"/>
+      <c r="BN50" s="192"/>
+      <c r="BO50" s="192"/>
+      <c r="BP50" s="192"/>
+      <c r="BQ50" s="193"/>
     </row>
     <row r="51" spans="1:69" s="50" customFormat="1">
       <c r="A51" s="52" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
-      <c r="B51" s="169" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="169"/>
-      <c r="D51" s="169"/>
-      <c r="E51" s="169"/>
-      <c r="F51" s="169"/>
-      <c r="G51" s="169"/>
-      <c r="H51" s="169"/>
-      <c r="I51" s="169"/>
-      <c r="J51" s="169"/>
-      <c r="K51" s="169"/>
-      <c r="L51" s="169"/>
-      <c r="M51" s="169"/>
-      <c r="N51" s="169"/>
-      <c r="O51" s="169"/>
-      <c r="P51" s="169"/>
-      <c r="Q51" s="169"/>
-      <c r="R51" s="169"/>
-      <c r="S51" s="169"/>
-      <c r="T51" s="169"/>
-      <c r="U51" s="169"/>
-      <c r="V51" s="169"/>
-      <c r="W51" s="169"/>
-      <c r="X51" s="169"/>
-      <c r="Y51" s="169"/>
-      <c r="Z51" s="169"/>
-      <c r="AA51" s="169"/>
-      <c r="AB51" s="169"/>
-      <c r="AC51" s="169"/>
-      <c r="AD51" s="169"/>
-      <c r="AE51" s="169"/>
-      <c r="AF51" s="169"/>
-      <c r="AG51" s="169"/>
-      <c r="AH51" s="169"/>
-      <c r="AI51" s="169"/>
-      <c r="AJ51" s="169"/>
-      <c r="AK51" s="169"/>
-      <c r="AL51" s="169"/>
-      <c r="AM51" s="169"/>
-      <c r="AN51" s="169"/>
-      <c r="AO51" s="169"/>
-      <c r="AP51" s="169"/>
-      <c r="AQ51" s="169"/>
-      <c r="AR51" s="169"/>
-      <c r="AS51" s="169"/>
-      <c r="AT51" s="169"/>
-      <c r="AU51" s="169"/>
-      <c r="AV51" s="169"/>
-      <c r="AW51" s="169"/>
-      <c r="AX51" s="169"/>
-      <c r="AY51" s="169"/>
-      <c r="AZ51" s="169"/>
-      <c r="BA51" s="169"/>
-      <c r="BB51" s="169"/>
-      <c r="BC51" s="169"/>
-      <c r="BD51" s="169"/>
-      <c r="BE51" s="169"/>
-      <c r="BF51" s="169"/>
-      <c r="BG51" s="169"/>
-      <c r="BH51" s="169"/>
-      <c r="BI51" s="169"/>
-      <c r="BJ51" s="169"/>
-      <c r="BK51" s="169"/>
-      <c r="BL51" s="169"/>
-      <c r="BM51" s="169"/>
-      <c r="BN51" s="169"/>
-      <c r="BO51" s="169"/>
-      <c r="BP51" s="169"/>
-      <c r="BQ51" s="170"/>
+      <c r="B51" s="194" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="194"/>
+      <c r="D51" s="194"/>
+      <c r="E51" s="194"/>
+      <c r="F51" s="194"/>
+      <c r="G51" s="194"/>
+      <c r="H51" s="194"/>
+      <c r="I51" s="194"/>
+      <c r="J51" s="194"/>
+      <c r="K51" s="194"/>
+      <c r="L51" s="194"/>
+      <c r="M51" s="194"/>
+      <c r="N51" s="194"/>
+      <c r="O51" s="194"/>
+      <c r="P51" s="194"/>
+      <c r="Q51" s="194"/>
+      <c r="R51" s="194"/>
+      <c r="S51" s="194"/>
+      <c r="T51" s="194"/>
+      <c r="U51" s="194"/>
+      <c r="V51" s="194"/>
+      <c r="W51" s="194"/>
+      <c r="X51" s="194"/>
+      <c r="Y51" s="194"/>
+      <c r="Z51" s="194"/>
+      <c r="AA51" s="194"/>
+      <c r="AB51" s="194"/>
+      <c r="AC51" s="194"/>
+      <c r="AD51" s="194"/>
+      <c r="AE51" s="194"/>
+      <c r="AF51" s="194"/>
+      <c r="AG51" s="194"/>
+      <c r="AH51" s="194"/>
+      <c r="AI51" s="194"/>
+      <c r="AJ51" s="194"/>
+      <c r="AK51" s="194"/>
+      <c r="AL51" s="194"/>
+      <c r="AM51" s="194"/>
+      <c r="AN51" s="194"/>
+      <c r="AO51" s="194"/>
+      <c r="AP51" s="194"/>
+      <c r="AQ51" s="194"/>
+      <c r="AR51" s="194"/>
+      <c r="AS51" s="194"/>
+      <c r="AT51" s="194"/>
+      <c r="AU51" s="194"/>
+      <c r="AV51" s="194"/>
+      <c r="AW51" s="194"/>
+      <c r="AX51" s="194"/>
+      <c r="AY51" s="194"/>
+      <c r="AZ51" s="194"/>
+      <c r="BA51" s="194"/>
+      <c r="BB51" s="194"/>
+      <c r="BC51" s="194"/>
+      <c r="BD51" s="194"/>
+      <c r="BE51" s="194"/>
+      <c r="BF51" s="194"/>
+      <c r="BG51" s="194"/>
+      <c r="BH51" s="194"/>
+      <c r="BI51" s="194"/>
+      <c r="BJ51" s="194"/>
+      <c r="BK51" s="194"/>
+      <c r="BL51" s="194"/>
+      <c r="BM51" s="194"/>
+      <c r="BN51" s="194"/>
+      <c r="BO51" s="194"/>
+      <c r="BP51" s="194"/>
+      <c r="BQ51" s="195"/>
     </row>
     <row r="52" spans="1:69" s="50" customFormat="1">
       <c r="A52" s="53" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
       </c>
-      <c r="B52" s="171" t="s">
-        <v>144</v>
-      </c>
-      <c r="C52" s="171"/>
-      <c r="D52" s="171"/>
-      <c r="E52" s="171"/>
-      <c r="F52" s="171"/>
-      <c r="G52" s="171"/>
-      <c r="H52" s="171"/>
-      <c r="I52" s="171"/>
-      <c r="J52" s="171"/>
-      <c r="K52" s="171"/>
-      <c r="L52" s="171"/>
-      <c r="M52" s="171"/>
-      <c r="N52" s="171"/>
-      <c r="O52" s="171"/>
-      <c r="P52" s="171"/>
-      <c r="Q52" s="171"/>
-      <c r="R52" s="171"/>
-      <c r="S52" s="171"/>
-      <c r="T52" s="171"/>
-      <c r="U52" s="171"/>
-      <c r="V52" s="171"/>
-      <c r="W52" s="171"/>
-      <c r="X52" s="171"/>
-      <c r="Y52" s="171"/>
-      <c r="Z52" s="171"/>
-      <c r="AA52" s="171"/>
-      <c r="AB52" s="171"/>
-      <c r="AC52" s="171"/>
-      <c r="AD52" s="171"/>
-      <c r="AE52" s="171"/>
-      <c r="AF52" s="171"/>
-      <c r="AG52" s="171"/>
-      <c r="AH52" s="171"/>
-      <c r="AI52" s="171"/>
-      <c r="AJ52" s="171"/>
-      <c r="AK52" s="171"/>
-      <c r="AL52" s="171"/>
-      <c r="AM52" s="171"/>
-      <c r="AN52" s="171"/>
-      <c r="AO52" s="171"/>
-      <c r="AP52" s="171"/>
-      <c r="AQ52" s="171"/>
-      <c r="AR52" s="171"/>
-      <c r="AS52" s="171"/>
-      <c r="AT52" s="171"/>
-      <c r="AU52" s="171"/>
-      <c r="AV52" s="171"/>
-      <c r="AW52" s="171"/>
-      <c r="AX52" s="171"/>
-      <c r="AY52" s="171"/>
-      <c r="AZ52" s="171"/>
-      <c r="BA52" s="171"/>
-      <c r="BB52" s="171"/>
-      <c r="BC52" s="171"/>
-      <c r="BD52" s="171"/>
-      <c r="BE52" s="171"/>
-      <c r="BF52" s="171"/>
-      <c r="BG52" s="171"/>
-      <c r="BH52" s="171"/>
-      <c r="BI52" s="171"/>
-      <c r="BJ52" s="171"/>
-      <c r="BK52" s="171"/>
-      <c r="BL52" s="171"/>
-      <c r="BM52" s="171"/>
-      <c r="BN52" s="171"/>
-      <c r="BO52" s="171"/>
-      <c r="BP52" s="171"/>
-      <c r="BQ52" s="172"/>
+      <c r="B52" s="196" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="196"/>
+      <c r="D52" s="196"/>
+      <c r="E52" s="196"/>
+      <c r="F52" s="196"/>
+      <c r="G52" s="196"/>
+      <c r="H52" s="196"/>
+      <c r="I52" s="196"/>
+      <c r="J52" s="196"/>
+      <c r="K52" s="196"/>
+      <c r="L52" s="196"/>
+      <c r="M52" s="196"/>
+      <c r="N52" s="196"/>
+      <c r="O52" s="196"/>
+      <c r="P52" s="196"/>
+      <c r="Q52" s="196"/>
+      <c r="R52" s="196"/>
+      <c r="S52" s="196"/>
+      <c r="T52" s="196"/>
+      <c r="U52" s="196"/>
+      <c r="V52" s="196"/>
+      <c r="W52" s="196"/>
+      <c r="X52" s="196"/>
+      <c r="Y52" s="196"/>
+      <c r="Z52" s="196"/>
+      <c r="AA52" s="196"/>
+      <c r="AB52" s="196"/>
+      <c r="AC52" s="196"/>
+      <c r="AD52" s="196"/>
+      <c r="AE52" s="196"/>
+      <c r="AF52" s="196"/>
+      <c r="AG52" s="196"/>
+      <c r="AH52" s="196"/>
+      <c r="AI52" s="196"/>
+      <c r="AJ52" s="196"/>
+      <c r="AK52" s="196"/>
+      <c r="AL52" s="196"/>
+      <c r="AM52" s="196"/>
+      <c r="AN52" s="196"/>
+      <c r="AO52" s="196"/>
+      <c r="AP52" s="196"/>
+      <c r="AQ52" s="196"/>
+      <c r="AR52" s="196"/>
+      <c r="AS52" s="196"/>
+      <c r="AT52" s="196"/>
+      <c r="AU52" s="196"/>
+      <c r="AV52" s="196"/>
+      <c r="AW52" s="196"/>
+      <c r="AX52" s="196"/>
+      <c r="AY52" s="196"/>
+      <c r="AZ52" s="196"/>
+      <c r="BA52" s="196"/>
+      <c r="BB52" s="196"/>
+      <c r="BC52" s="196"/>
+      <c r="BD52" s="196"/>
+      <c r="BE52" s="196"/>
+      <c r="BF52" s="196"/>
+      <c r="BG52" s="196"/>
+      <c r="BH52" s="196"/>
+      <c r="BI52" s="196"/>
+      <c r="BJ52" s="196"/>
+      <c r="BK52" s="196"/>
+      <c r="BL52" s="196"/>
+      <c r="BM52" s="196"/>
+      <c r="BN52" s="196"/>
+      <c r="BO52" s="196"/>
+      <c r="BP52" s="196"/>
+      <c r="BQ52" s="197"/>
     </row>
     <row r="53" spans="1:69" s="50" customFormat="1">
       <c r="A53" s="54" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
       </c>
-      <c r="B53" s="173" t="s">
-        <v>145</v>
-      </c>
-      <c r="C53" s="173"/>
-      <c r="D53" s="173"/>
-      <c r="E53" s="173"/>
-      <c r="F53" s="173"/>
-      <c r="G53" s="173"/>
-      <c r="H53" s="173"/>
-      <c r="I53" s="173"/>
-      <c r="J53" s="173"/>
-      <c r="K53" s="173"/>
-      <c r="L53" s="173"/>
-      <c r="M53" s="173"/>
-      <c r="N53" s="173"/>
-      <c r="O53" s="173"/>
-      <c r="P53" s="173"/>
-      <c r="Q53" s="173"/>
-      <c r="R53" s="173"/>
-      <c r="S53" s="173"/>
-      <c r="T53" s="173"/>
-      <c r="U53" s="173"/>
-      <c r="V53" s="173"/>
-      <c r="W53" s="173"/>
-      <c r="X53" s="173"/>
-      <c r="Y53" s="173"/>
-      <c r="Z53" s="173"/>
-      <c r="AA53" s="173"/>
-      <c r="AB53" s="173"/>
-      <c r="AC53" s="173"/>
-      <c r="AD53" s="173"/>
-      <c r="AE53" s="173"/>
-      <c r="AF53" s="173"/>
-      <c r="AG53" s="173"/>
-      <c r="AH53" s="173"/>
-      <c r="AI53" s="173"/>
-      <c r="AJ53" s="173"/>
-      <c r="AK53" s="173"/>
-      <c r="AL53" s="173"/>
-      <c r="AM53" s="173"/>
-      <c r="AN53" s="173"/>
-      <c r="AO53" s="173"/>
-      <c r="AP53" s="173"/>
-      <c r="AQ53" s="173"/>
-      <c r="AR53" s="173"/>
-      <c r="AS53" s="173"/>
-      <c r="AT53" s="173"/>
-      <c r="AU53" s="173"/>
-      <c r="AV53" s="173"/>
-      <c r="AW53" s="173"/>
-      <c r="AX53" s="173"/>
-      <c r="AY53" s="173"/>
-      <c r="AZ53" s="173"/>
-      <c r="BA53" s="173"/>
-      <c r="BB53" s="173"/>
-      <c r="BC53" s="173"/>
-      <c r="BD53" s="173"/>
-      <c r="BE53" s="173"/>
-      <c r="BF53" s="173"/>
-      <c r="BG53" s="173"/>
-      <c r="BH53" s="173"/>
-      <c r="BI53" s="173"/>
-      <c r="BJ53" s="173"/>
-      <c r="BK53" s="173"/>
-      <c r="BL53" s="173"/>
-      <c r="BM53" s="173"/>
-      <c r="BN53" s="173"/>
-      <c r="BO53" s="173"/>
-      <c r="BP53" s="173"/>
-      <c r="BQ53" s="174"/>
+      <c r="B53" s="198" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="198"/>
+      <c r="D53" s="198"/>
+      <c r="E53" s="198"/>
+      <c r="F53" s="198"/>
+      <c r="G53" s="198"/>
+      <c r="H53" s="198"/>
+      <c r="I53" s="198"/>
+      <c r="J53" s="198"/>
+      <c r="K53" s="198"/>
+      <c r="L53" s="198"/>
+      <c r="M53" s="198"/>
+      <c r="N53" s="198"/>
+      <c r="O53" s="198"/>
+      <c r="P53" s="198"/>
+      <c r="Q53" s="198"/>
+      <c r="R53" s="198"/>
+      <c r="S53" s="198"/>
+      <c r="T53" s="198"/>
+      <c r="U53" s="198"/>
+      <c r="V53" s="198"/>
+      <c r="W53" s="198"/>
+      <c r="X53" s="198"/>
+      <c r="Y53" s="198"/>
+      <c r="Z53" s="198"/>
+      <c r="AA53" s="198"/>
+      <c r="AB53" s="198"/>
+      <c r="AC53" s="198"/>
+      <c r="AD53" s="198"/>
+      <c r="AE53" s="198"/>
+      <c r="AF53" s="198"/>
+      <c r="AG53" s="198"/>
+      <c r="AH53" s="198"/>
+      <c r="AI53" s="198"/>
+      <c r="AJ53" s="198"/>
+      <c r="AK53" s="198"/>
+      <c r="AL53" s="198"/>
+      <c r="AM53" s="198"/>
+      <c r="AN53" s="198"/>
+      <c r="AO53" s="198"/>
+      <c r="AP53" s="198"/>
+      <c r="AQ53" s="198"/>
+      <c r="AR53" s="198"/>
+      <c r="AS53" s="198"/>
+      <c r="AT53" s="198"/>
+      <c r="AU53" s="198"/>
+      <c r="AV53" s="198"/>
+      <c r="AW53" s="198"/>
+      <c r="AX53" s="198"/>
+      <c r="AY53" s="198"/>
+      <c r="AZ53" s="198"/>
+      <c r="BA53" s="198"/>
+      <c r="BB53" s="198"/>
+      <c r="BC53" s="198"/>
+      <c r="BD53" s="198"/>
+      <c r="BE53" s="198"/>
+      <c r="BF53" s="198"/>
+      <c r="BG53" s="198"/>
+      <c r="BH53" s="198"/>
+      <c r="BI53" s="198"/>
+      <c r="BJ53" s="198"/>
+      <c r="BK53" s="198"/>
+      <c r="BL53" s="198"/>
+      <c r="BM53" s="198"/>
+      <c r="BN53" s="198"/>
+      <c r="BO53" s="198"/>
+      <c r="BP53" s="198"/>
+      <c r="BQ53" s="199"/>
     </row>
     <row r="54" spans="1:69">
       <c r="A54" s="54" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.4</v>
       </c>
-      <c r="B54" s="173" t="s">
-        <v>146</v>
-      </c>
-      <c r="C54" s="173"/>
-      <c r="D54" s="173"/>
-      <c r="E54" s="173"/>
-      <c r="F54" s="173"/>
-      <c r="G54" s="173"/>
-      <c r="H54" s="173"/>
-      <c r="I54" s="173"/>
-      <c r="J54" s="173"/>
-      <c r="K54" s="173"/>
-      <c r="L54" s="173"/>
-      <c r="M54" s="173"/>
-      <c r="N54" s="173"/>
-      <c r="O54" s="173"/>
-      <c r="P54" s="173"/>
-      <c r="Q54" s="173"/>
-      <c r="R54" s="173"/>
-      <c r="S54" s="173"/>
-      <c r="T54" s="173"/>
-      <c r="U54" s="173"/>
-      <c r="V54" s="173"/>
-      <c r="W54" s="173"/>
-      <c r="X54" s="173"/>
-      <c r="Y54" s="173"/>
-      <c r="Z54" s="173"/>
-      <c r="AA54" s="173"/>
-      <c r="AB54" s="173"/>
-      <c r="AC54" s="173"/>
-      <c r="AD54" s="173"/>
-      <c r="AE54" s="173"/>
-      <c r="AF54" s="173"/>
-      <c r="AG54" s="173"/>
-      <c r="AH54" s="173"/>
-      <c r="AI54" s="173"/>
-      <c r="AJ54" s="173"/>
-      <c r="AK54" s="173"/>
-      <c r="AL54" s="173"/>
-      <c r="AM54" s="173"/>
-      <c r="AN54" s="173"/>
-      <c r="AO54" s="173"/>
-      <c r="AP54" s="173"/>
-      <c r="AQ54" s="173"/>
-      <c r="AR54" s="173"/>
-      <c r="AS54" s="173"/>
-      <c r="AT54" s="173"/>
-      <c r="AU54" s="173"/>
-      <c r="AV54" s="173"/>
-      <c r="AW54" s="173"/>
-      <c r="AX54" s="173"/>
-      <c r="AY54" s="173"/>
-      <c r="AZ54" s="173"/>
-      <c r="BA54" s="173"/>
-      <c r="BB54" s="173"/>
-      <c r="BC54" s="173"/>
-      <c r="BD54" s="173"/>
-      <c r="BE54" s="173"/>
-      <c r="BF54" s="173"/>
-      <c r="BG54" s="173"/>
-      <c r="BH54" s="173"/>
-      <c r="BI54" s="173"/>
-      <c r="BJ54" s="173"/>
-      <c r="BK54" s="173"/>
-      <c r="BL54" s="173"/>
-      <c r="BM54" s="173"/>
-      <c r="BN54" s="173"/>
-      <c r="BO54" s="173"/>
-      <c r="BP54" s="173"/>
-      <c r="BQ54" s="174"/>
+      <c r="B54" s="198" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="198"/>
+      <c r="D54" s="198"/>
+      <c r="E54" s="198"/>
+      <c r="F54" s="198"/>
+      <c r="G54" s="198"/>
+      <c r="H54" s="198"/>
+      <c r="I54" s="198"/>
+      <c r="J54" s="198"/>
+      <c r="K54" s="198"/>
+      <c r="L54" s="198"/>
+      <c r="M54" s="198"/>
+      <c r="N54" s="198"/>
+      <c r="O54" s="198"/>
+      <c r="P54" s="198"/>
+      <c r="Q54" s="198"/>
+      <c r="R54" s="198"/>
+      <c r="S54" s="198"/>
+      <c r="T54" s="198"/>
+      <c r="U54" s="198"/>
+      <c r="V54" s="198"/>
+      <c r="W54" s="198"/>
+      <c r="X54" s="198"/>
+      <c r="Y54" s="198"/>
+      <c r="Z54" s="198"/>
+      <c r="AA54" s="198"/>
+      <c r="AB54" s="198"/>
+      <c r="AC54" s="198"/>
+      <c r="AD54" s="198"/>
+      <c r="AE54" s="198"/>
+      <c r="AF54" s="198"/>
+      <c r="AG54" s="198"/>
+      <c r="AH54" s="198"/>
+      <c r="AI54" s="198"/>
+      <c r="AJ54" s="198"/>
+      <c r="AK54" s="198"/>
+      <c r="AL54" s="198"/>
+      <c r="AM54" s="198"/>
+      <c r="AN54" s="198"/>
+      <c r="AO54" s="198"/>
+      <c r="AP54" s="198"/>
+      <c r="AQ54" s="198"/>
+      <c r="AR54" s="198"/>
+      <c r="AS54" s="198"/>
+      <c r="AT54" s="198"/>
+      <c r="AU54" s="198"/>
+      <c r="AV54" s="198"/>
+      <c r="AW54" s="198"/>
+      <c r="AX54" s="198"/>
+      <c r="AY54" s="198"/>
+      <c r="AZ54" s="198"/>
+      <c r="BA54" s="198"/>
+      <c r="BB54" s="198"/>
+      <c r="BC54" s="198"/>
+      <c r="BD54" s="198"/>
+      <c r="BE54" s="198"/>
+      <c r="BF54" s="198"/>
+      <c r="BG54" s="198"/>
+      <c r="BH54" s="198"/>
+      <c r="BI54" s="198"/>
+      <c r="BJ54" s="198"/>
+      <c r="BK54" s="198"/>
+      <c r="BL54" s="198"/>
+      <c r="BM54" s="198"/>
+      <c r="BN54" s="198"/>
+      <c r="BO54" s="198"/>
+      <c r="BP54" s="198"/>
+      <c r="BQ54" s="199"/>
     </row>
     <row r="55" spans="1:69" s="50" customFormat="1">
       <c r="A55" s="51" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
-      <c r="B55" s="167" t="s">
-        <v>147</v>
-      </c>
-      <c r="C55" s="167"/>
-      <c r="D55" s="167"/>
-      <c r="E55" s="167"/>
-      <c r="F55" s="167"/>
-      <c r="G55" s="167"/>
-      <c r="H55" s="167"/>
-      <c r="I55" s="167"/>
-      <c r="J55" s="167"/>
-      <c r="K55" s="167"/>
-      <c r="L55" s="167"/>
-      <c r="M55" s="167"/>
-      <c r="N55" s="167"/>
-      <c r="O55" s="167"/>
-      <c r="P55" s="167"/>
-      <c r="Q55" s="167"/>
-      <c r="R55" s="167"/>
-      <c r="S55" s="167"/>
-      <c r="T55" s="167"/>
-      <c r="U55" s="167"/>
-      <c r="V55" s="167"/>
-      <c r="W55" s="167"/>
-      <c r="X55" s="167"/>
-      <c r="Y55" s="167"/>
-      <c r="Z55" s="167"/>
-      <c r="AA55" s="167"/>
-      <c r="AB55" s="167"/>
-      <c r="AC55" s="167"/>
-      <c r="AD55" s="167"/>
-      <c r="AE55" s="167"/>
-      <c r="AF55" s="167"/>
-      <c r="AG55" s="167"/>
-      <c r="AH55" s="167"/>
-      <c r="AI55" s="167"/>
-      <c r="AJ55" s="167"/>
-      <c r="AK55" s="167"/>
-      <c r="AL55" s="167"/>
-      <c r="AM55" s="167"/>
-      <c r="AN55" s="167"/>
-      <c r="AO55" s="167"/>
-      <c r="AP55" s="167"/>
-      <c r="AQ55" s="167"/>
-      <c r="AR55" s="167"/>
-      <c r="AS55" s="167"/>
-      <c r="AT55" s="167"/>
-      <c r="AU55" s="167"/>
-      <c r="AV55" s="167"/>
-      <c r="AW55" s="167"/>
-      <c r="AX55" s="167"/>
-      <c r="AY55" s="167"/>
-      <c r="AZ55" s="167"/>
-      <c r="BA55" s="167"/>
-      <c r="BB55" s="167"/>
-      <c r="BC55" s="167"/>
-      <c r="BD55" s="167"/>
-      <c r="BE55" s="167"/>
-      <c r="BF55" s="167"/>
-      <c r="BG55" s="167"/>
-      <c r="BH55" s="167"/>
-      <c r="BI55" s="167"/>
-      <c r="BJ55" s="167"/>
-      <c r="BK55" s="167"/>
-      <c r="BL55" s="167"/>
-      <c r="BM55" s="167"/>
-      <c r="BN55" s="167"/>
-      <c r="BO55" s="167"/>
-      <c r="BP55" s="167"/>
-      <c r="BQ55" s="168"/>
+      <c r="B55" s="192" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="192"/>
+      <c r="D55" s="192"/>
+      <c r="E55" s="192"/>
+      <c r="F55" s="192"/>
+      <c r="G55" s="192"/>
+      <c r="H55" s="192"/>
+      <c r="I55" s="192"/>
+      <c r="J55" s="192"/>
+      <c r="K55" s="192"/>
+      <c r="L55" s="192"/>
+      <c r="M55" s="192"/>
+      <c r="N55" s="192"/>
+      <c r="O55" s="192"/>
+      <c r="P55" s="192"/>
+      <c r="Q55" s="192"/>
+      <c r="R55" s="192"/>
+      <c r="S55" s="192"/>
+      <c r="T55" s="192"/>
+      <c r="U55" s="192"/>
+      <c r="V55" s="192"/>
+      <c r="W55" s="192"/>
+      <c r="X55" s="192"/>
+      <c r="Y55" s="192"/>
+      <c r="Z55" s="192"/>
+      <c r="AA55" s="192"/>
+      <c r="AB55" s="192"/>
+      <c r="AC55" s="192"/>
+      <c r="AD55" s="192"/>
+      <c r="AE55" s="192"/>
+      <c r="AF55" s="192"/>
+      <c r="AG55" s="192"/>
+      <c r="AH55" s="192"/>
+      <c r="AI55" s="192"/>
+      <c r="AJ55" s="192"/>
+      <c r="AK55" s="192"/>
+      <c r="AL55" s="192"/>
+      <c r="AM55" s="192"/>
+      <c r="AN55" s="192"/>
+      <c r="AO55" s="192"/>
+      <c r="AP55" s="192"/>
+      <c r="AQ55" s="192"/>
+      <c r="AR55" s="192"/>
+      <c r="AS55" s="192"/>
+      <c r="AT55" s="192"/>
+      <c r="AU55" s="192"/>
+      <c r="AV55" s="192"/>
+      <c r="AW55" s="192"/>
+      <c r="AX55" s="192"/>
+      <c r="AY55" s="192"/>
+      <c r="AZ55" s="192"/>
+      <c r="BA55" s="192"/>
+      <c r="BB55" s="192"/>
+      <c r="BC55" s="192"/>
+      <c r="BD55" s="192"/>
+      <c r="BE55" s="192"/>
+      <c r="BF55" s="192"/>
+      <c r="BG55" s="192"/>
+      <c r="BH55" s="192"/>
+      <c r="BI55" s="192"/>
+      <c r="BJ55" s="192"/>
+      <c r="BK55" s="192"/>
+      <c r="BL55" s="192"/>
+      <c r="BM55" s="192"/>
+      <c r="BN55" s="192"/>
+      <c r="BO55" s="192"/>
+      <c r="BP55" s="192"/>
+      <c r="BQ55" s="193"/>
     </row>
     <row r="56" spans="1:69" s="50" customFormat="1">
       <c r="A56" s="52" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B56" s="127" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C56" s="127"/>
       <c r="D56" s="127"/>
@@ -9074,11 +9055,11 @@
     </row>
     <row r="57" spans="1:69" s="50" customFormat="1">
       <c r="A57" s="53" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
       </c>
       <c r="B57" s="129" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C57" s="129"/>
       <c r="D57" s="129"/>
@@ -9150,11 +9131,11 @@
     </row>
     <row r="58" spans="1:69" s="50" customFormat="1">
       <c r="A58" s="53" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
       </c>
       <c r="B58" s="129" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C58" s="129"/>
       <c r="D58" s="129"/>
@@ -9226,11 +9207,11 @@
     </row>
     <row r="59" spans="1:69" s="50" customFormat="1" ht="17.25" customHeight="1">
       <c r="A59" s="53" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
       </c>
       <c r="B59" s="129" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C59" s="129"/>
       <c r="D59" s="129"/>
@@ -9302,11 +9283,11 @@
     </row>
     <row r="60" spans="1:69" s="50" customFormat="1">
       <c r="A60" s="51" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
       <c r="B60" s="131" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C60" s="131"/>
       <c r="D60" s="131"/>
@@ -9378,11 +9359,11 @@
     </row>
     <row r="61" spans="1:69" s="50" customFormat="1">
       <c r="A61" s="52" t="str">
-        <f t="shared" ref="A61:A64" ca="1" si="48">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A61:A64" si="48">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B61" s="127" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C61" s="127"/>
       <c r="D61" s="127"/>
@@ -9454,11 +9435,11 @@
     </row>
     <row r="62" spans="1:69" s="50" customFormat="1">
       <c r="A62" s="53" t="str">
-        <f t="shared" ca="1" si="48"/>
+        <f t="shared" si="48"/>
         <v>3.2</v>
       </c>
       <c r="B62" s="129" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C62" s="129"/>
       <c r="D62" s="129"/>
@@ -9530,11 +9511,11 @@
     </row>
     <row r="63" spans="1:69" s="50" customFormat="1">
       <c r="A63" s="53" t="str">
-        <f t="shared" ca="1" si="48"/>
+        <f t="shared" si="48"/>
         <v>3.3</v>
       </c>
       <c r="B63" s="129" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C63" s="129"/>
       <c r="D63" s="129"/>
@@ -9606,11 +9587,11 @@
     </row>
     <row r="64" spans="1:69" s="50" customFormat="1">
       <c r="A64" s="53" t="str">
-        <f t="shared" ca="1" si="48"/>
+        <f t="shared" si="48"/>
         <v>3.4</v>
       </c>
       <c r="B64" s="129" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C64" s="129"/>
       <c r="D64" s="129"/>
@@ -9696,14 +9677,20 @@
     <row r="78"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A11:L48" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A11:L48" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="I"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="28">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="N8:T8"/>
-    <mergeCell ref="U8:AA8"/>
-    <mergeCell ref="AB8:AH8"/>
-    <mergeCell ref="AI8:AO8"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B50:BQ50"/>
+    <mergeCell ref="B51:BQ51"/>
+    <mergeCell ref="B52:BQ52"/>
+    <mergeCell ref="B53:BQ53"/>
+    <mergeCell ref="B55:BQ55"/>
+    <mergeCell ref="B54:BQ54"/>
     <mergeCell ref="A1:BQ1"/>
     <mergeCell ref="A2:BQ2"/>
     <mergeCell ref="A3:BQ3"/>
@@ -9720,12 +9707,12 @@
     <mergeCell ref="AB9:AH9"/>
     <mergeCell ref="AI9:AO9"/>
     <mergeCell ref="AP9:AV9"/>
-    <mergeCell ref="B50:BQ50"/>
-    <mergeCell ref="B51:BQ51"/>
-    <mergeCell ref="B52:BQ52"/>
-    <mergeCell ref="B53:BQ53"/>
-    <mergeCell ref="B55:BQ55"/>
-    <mergeCell ref="B54:BQ54"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="N8:T8"/>
+    <mergeCell ref="U8:AA8"/>
+    <mergeCell ref="AB8:AH8"/>
+    <mergeCell ref="AI8:AO8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="L12:L13 L46 L25 L15:L16 L21:L22 L39:L40 L32 L27:L30 L42:L43">
     <cfRule type="dataBar" priority="182">
@@ -10141,15 +10128,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>68580</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>30</xdr:col>
-                    <xdr:colOff>137160</xdr:colOff>
+                    <xdr:col>22</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>53340</xdr:rowOff>
+                    <xdr:rowOff>57150</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10472,67 +10459,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="175"/>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-    </row>
-    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A2" s="176" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-    </row>
-    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A3" s="176" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
+      <c r="A1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+    </row>
+    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A2" s="187" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+    </row>
+    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A3" s="187" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="187"/>
+      <c r="P3" s="187"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="126"/>
@@ -10552,7 +10541,7 @@
       <c r="O4" s="126"/>
       <c r="P4" s="126"/>
     </row>
-    <row r="5" spans="1:16" ht="14.45" thickTop="1"/>
+    <row r="5" spans="1:16" ht="17.25" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
@@ -10570,67 +10559,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="175"/>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-    </row>
-    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A2" s="176" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-    </row>
-    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A3" s="176" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
+      <c r="A1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+    </row>
+    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A2" s="187" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+    </row>
+    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A3" s="187" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="187"/>
+      <c r="P3" s="187"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="126"/>
@@ -10650,7 +10641,7 @@
       <c r="O4" s="126"/>
       <c r="P4" s="126"/>
     </row>
-    <row r="5" spans="1:16" ht="14.45" thickTop="1"/>
+    <row r="5" spans="1:16" ht="17.25" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
@@ -10668,67 +10659,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="175"/>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-    </row>
-    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A2" s="176" t="s">
+      <c r="A1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+    </row>
+    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A2" s="187" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+    </row>
+    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A3" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-    </row>
-    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A3" s="176" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="187"/>
+      <c r="P3" s="187"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="126"/>
@@ -10748,7 +10741,7 @@
       <c r="O4" s="126"/>
       <c r="P4" s="126"/>
     </row>
-    <row r="5" spans="1:16" ht="14.45" thickTop="1"/>
+    <row r="5" spans="1:16" ht="17.25" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
@@ -10766,67 +10759,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="175"/>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-    </row>
-    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A2" s="176" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-    </row>
-    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.45">
-      <c r="A3" s="176" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
+      <c r="A1" s="186"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="186"/>
+    </row>
+    <row r="2" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A2" s="187" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+    </row>
+    <row r="3" spans="1:16" s="60" customFormat="1" ht="20.25">
+      <c r="A3" s="187" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="187"/>
+      <c r="P3" s="187"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="126"/>
@@ -10846,7 +10841,7 @@
       <c r="O4" s="126"/>
       <c r="P4" s="126"/>
     </row>
-    <row r="5" spans="1:16" ht="14.45" thickTop="1"/>
+    <row r="5" spans="1:16" ht="17.25" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:M1"/>

</xml_diff>